<commit_message>
update Story Points Excel
</commit_message>
<xml_diff>
--- a/docs/Overview_Story_Points_Volatility.xlsx
+++ b/docs/Overview_Story_Points_Volatility.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sophi\Winfo\5\WI-Projekt\bsi-projekt-ws22-tbc\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A134D352-D361-4673-9954-E78818C4AC25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D345B6-0E82-487B-851B-122B05D43C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{44DE59B5-FEC1-4B06-9D73-FC017AEBA9CC}"/>
+    <workbookView xWindow="22020" yWindow="4695" windowWidth="16560" windowHeight="15225" xr2:uid="{44DE59B5-FEC1-4B06-9D73-FC017AEBA9CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>fertig</t>
   </si>
 </sst>
 </file>
@@ -569,19 +572,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C1ECC9E-B7F1-421F-9262-F56082CEAD5C}">
   <dimension ref="A5:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="38.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -601,7 +604,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -615,7 +618,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -629,7 +632,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -646,7 +649,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -656,8 +659,11 @@
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
@@ -674,7 +680,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -691,7 +697,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
@@ -708,7 +714,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>26</v>
       </c>
@@ -725,7 +731,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
@@ -742,7 +748,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>16</v>
       </c>
@@ -759,7 +765,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>23</v>
       </c>
@@ -776,7 +782,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>24</v>
       </c>
@@ -790,10 +796,10 @@
         <v>13</v>
       </c>
       <c r="F17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>13</v>
       </c>
@@ -807,10 +813,10 @@
         <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>19</v>
       </c>
@@ -824,7 +830,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>11</v>
       </c>
@@ -838,22 +844,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>20</v>
       </c>
@@ -864,7 +870,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>21</v>
       </c>
@@ -875,7 +881,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>13</v>
       </c>
@@ -886,7 +892,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E28" s="4">
         <v>20</v>
       </c>
@@ -894,7 +900,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E29" s="4">
         <v>5</v>
       </c>
@@ -902,7 +908,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E30" s="4">
         <v>8</v>
       </c>
@@ -910,7 +916,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E31" s="4">
         <v>5</v>
       </c>
@@ -918,7 +924,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E32" s="4">
         <v>13</v>
       </c>
@@ -926,7 +932,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E33" s="11">
         <v>3</v>
       </c>
@@ -934,13 +940,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E34" s="4">
         <f>SUM(E26:E33)</f>
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E37" s="14" t="s">
         <v>22</v>
       </c>
@@ -954,7 +960,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
         <v>30</v>
       </c>
@@ -962,7 +968,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E39" t="s">
         <v>31</v>
       </c>
@@ -970,7 +976,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E40" t="s">
         <v>32</v>
       </c>
@@ -978,7 +984,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
         <v>35</v>
       </c>
@@ -986,7 +992,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="5:9" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
         <v>25</v>
       </c>
@@ -1001,7 +1007,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="5:9" x14ac:dyDescent="0.25">
       <c r="F43" t="s">
         <v>33</v>
       </c>
@@ -1010,7 +1016,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="5:9" x14ac:dyDescent="0.25">
       <c r="F44" t="s">
         <v>34</v>
       </c>
@@ -1019,7 +1025,7 @@
         <v>0.61038961038961037</v>
       </c>
     </row>
-    <row r="47" spans="5:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="5:9" x14ac:dyDescent="0.25">
       <c r="F47" s="12" t="s">
         <v>36</v>
       </c>

</xml_diff>